<commit_message>
Manual Testing XLSX File
</commit_message>
<xml_diff>
--- a/Manual Testing (QA 181).xlsx
+++ b/Manual Testing (QA 181).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C48D7975-D7B7-4C0A-8441-B4642291DF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1037EC67-4F4F-4735-A81A-7532B21D0D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5A5855E8-DC13-4342-B4E6-BC4307752C68}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>Project Name:</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Actual Result</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
   <si>
     <t>Executed By</t>
@@ -176,7 +173,41 @@
     <t>Message box got displayed</t>
   </si>
   <si>
-    <t>Fail</t>
+    <t>Enter a valid username &amp; an invalid password</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_003</t>
+  </si>
+  <si>
+    <t>Enter an invalid username &amp; a valid password</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter valid password
+3. Click on the login button</t>
+  </si>
+  <si>
+    <t>Username: xxxxx@erp.com
+Password: P@ssw0rd</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_004</t>
+  </si>
+  <si>
+    <t>Enter an invalid username &amp; an invalid password</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter an invalid password
+3. Click on the login button</t>
+  </si>
+  <si>
+    <t>Username: xxxxx@erp.com
+Password: xxxxxxxxx</t>
+  </si>
+  <si>
+    <t>Test Case 
+Status</t>
   </si>
 </sst>
 </file>
@@ -186,7 +217,7 @@
   <numFmts count="1">
     <numFmt numFmtId="166" formatCode="dd/mmm/yyyy\ \(ddd\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,16 +233,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -220,25 +291,156 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -246,23 +448,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,11 +819,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A49120B-495C-41A7-B2B9-723AFDE227B5}">
-  <dimension ref="A2:N13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -600,217 +840,275 @@
     <col min="14" max="14" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="22">
         <v>44977</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="23">
         <v>45003</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1" ht="131" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="B10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="13">
+        <v>44979</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" s="2" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+    <row r="11" spans="1:14" ht="131" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="7" t="s">
+      <c r="G11" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="L11" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="M11" s="18">
+        <v>44982</v>
+      </c>
+      <c r="N11" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M10" s="8">
-        <v>44979</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="11" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+    <row r="12" spans="1:14" ht="131" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="G12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="I12" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="J12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="6" t="s">
+      <c r="K12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="13">
+        <v>44984</v>
+      </c>
+      <c r="N12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="M11" s="8">
-        <v>44982</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
+    <row r="13" spans="1:14" ht="131" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="18">
+        <v>44988</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>